<commit_message>
refactor pledge subject service & enums
</commit_message>
<xml_diff>
--- a/src/test/java/ru/fds/tavrzcms3/testdata/pledge_subject_auto_new.xlsx
+++ b/src/test/java/ru/fds/tavrzcms3/testdata/pledge_subject_auto_new.xlsx
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>